<commit_message>
Ranking y guardar puntakes
</commit_message>
<xml_diff>
--- a/src/files/Ranking.xlsx
+++ b/src/files/Ranking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arang\Downloads\ProyectoFinalPoo\src\files\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>AlexanderRV</t>
   </si>
@@ -84,12 +84,16 @@
   </si>
   <si>
     <t>SaraL</t>
+  </si>
+  <si>
+    <t>Judith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -472,153 +476,161 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>800</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>750</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>700</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>650</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>600</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>550</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>500</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>450</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>400</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>350</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>300</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>250</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>0</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>150</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>100</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>50</v>
       </c>
       <c r="E16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n" s="0">
+        <v>650.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios de explanation and puntaje
</commit_message>
<xml_diff>
--- a/src/files/Ranking.xlsx
+++ b/src/files/Ranking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arang\Downloads\ProyectoFinalPoo\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A90D31B-58E5-4FA2-AF9F-DCD2D90DE01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECAEDF3-E618-4604-B634-F23F5758A3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="150" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>AlexanderRV</t>
   </si>
@@ -87,6 +87,66 @@
   </si>
   <si>
     <t>Judith</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>ola</t>
+  </si>
+  <si>
+    <t>lacrespa</t>
+  </si>
+  <si>
+    <t>Daddy Yankee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUlip </t>
+  </si>
+  <si>
+    <t>Bryant Myers</t>
+  </si>
+  <si>
+    <t>Margarita</t>
+  </si>
+  <si>
+    <t>miku</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>ale</t>
+  </si>
+  <si>
+    <t>Elvi</t>
+  </si>
+  <si>
+    <t>camilo</t>
+  </si>
+  <si>
+    <t>Clubpinguin69</t>
+  </si>
+  <si>
+    <t>Jose :3</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>crisd</t>
+  </si>
+  <si>
+    <t>Mery</t>
   </si>
 </sst>
 </file>
@@ -468,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,12 +684,188 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B17" t="n" s="0">
-        <v>650.0</v>
+      <c r="B17" s="0">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n" s="0">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n" s="0">
+        <v>1300.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n" s="0">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B30" t="n" s="0">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n" s="0">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n" s="0">
+        <v>800.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n" s="0">
+        <v>850.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n" s="0">
+        <v>850.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n" s="0">
+        <v>1250.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n" s="0">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n" s="0">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n" s="0">
+        <v>1300.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B39" t="n" s="0">
+        <v>700.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>